<commit_message>
adjsutments on the boosted Daily rewards
Former-commit-id: b351bcea7fb36e4e86841d82f2fbd944d1958969
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
+++ b/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I23" s="8">
         <v>0</v>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I25" s="8">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         <v>82</v>
       </c>
       <c r="H26" s="8">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="I26" s="8">
         <v>0</v>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="8">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I27" s="8">
         <v>0</v>
@@ -1635,5 +1635,6 @@
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5 D22:D28 D42:D45 D36 D11:D16"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added minRuns 4 to welcome back feature
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
+++ b/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdiez\Documents\client_lfs\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15960"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="18360" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>egg_dailyLogin_baby_welcomeBack</t>
+  </si>
+  <si>
+    <t>[minRuns]</t>
   </si>
 </sst>
 </file>
@@ -791,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N45"/>
+  <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,13 +811,14 @@
     <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
@@ -826,7 +830,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="4" spans="2:14" ht="170.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="170.25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
@@ -837,37 +841,40 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -878,38 +885,41 @@
         <v>1</v>
       </c>
       <c r="E5" s="8">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8">
         <v>14</v>
       </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>7</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>12</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>1000</v>
       </c>
-      <c r="M5" s="8">
+      <c r="N5" s="8">
         <v>3</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -921,7 +931,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="10" spans="2:14" s="17" customFormat="1" ht="152.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" s="17" customFormat="1" ht="152.25" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>76</v>
       </c>
@@ -962,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Adjustments on content Welcome: - Changed Solo Quest efinition: goals, Quest type to Fire Rushes and Jalapeno_invasion mod [sku] solo_quest_fire_rush  [type] fire_rush  [target] [icon]  icon_firerush [amount] 32  [duration]  10080  [description]  TID_GLOBAL_EVENT_FIRERUSH
- Changed WELCOME BACK DEFINITIONS
[passiveDurationDays] 7
[passiveModSku] jalapeno_invasion
[tournamentPassDurationHours] 10080 (7days)
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
+++ b/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -65,9 +65,6 @@
     <t>[minAbsentDays]</t>
   </si>
   <si>
-    <t>solo_quest_birds</t>
-  </si>
-  <si>
     <t>[soloQuestSku]</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>[passiveModSku]</t>
   </si>
   <si>
-    <t>midas</t>
-  </si>
-  <si>
     <t>[tournamentPassDurationHours]</t>
   </si>
   <si>
@@ -113,18 +107,6 @@
     <t>[description]</t>
   </si>
   <si>
-    <t>kill</t>
-  </si>
-  <si>
-    <t>Canary01_Flock;Canary02_Flock;Canary03_Flock;Canary04_Flock</t>
-  </si>
-  <si>
-    <t>icon_canary</t>
-  </si>
-  <si>
-    <t>TID_GLOBAL_EVENT_SPACE_BIRD</t>
-  </si>
-  <si>
     <t>[maxActivationsAllowed]</t>
   </si>
   <si>
@@ -279,6 +261,21 @@
   </si>
   <si>
     <t>[minRuns]</t>
+  </si>
+  <si>
+    <t>solo_quest_fire_rush</t>
+  </si>
+  <si>
+    <t>fire_rush</t>
+  </si>
+  <si>
+    <t>icon_firerush</t>
+  </si>
+  <si>
+    <t>TID_GLOBAL_EVENT_FIRERUSH</t>
+  </si>
+  <si>
+    <t>jalapeno_invasion</t>
   </si>
 </sst>
 </file>
@@ -324,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +364,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -450,11 +453,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,6 +521,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +844,7 @@
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -832,7 +856,7 @@
     </row>
     <row r="4" spans="2:15" ht="170.25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -841,40 +865,40 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -893,35 +917,35 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>12</v>
+      <c r="H5" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="I5" s="8">
         <v>7</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>16</v>
+      <c r="J5" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="K5" s="8">
-        <v>12</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>5</v>
+        <v>10080</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
       </c>
       <c r="M5" s="8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N5" s="8">
         <v>3</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -933,7 +957,7 @@
     </row>
     <row r="10" spans="2:15" s="17" customFormat="1" ht="152.25" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>2</v>
@@ -942,34 +966,34 @@
         <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="J10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -977,16 +1001,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="b">
@@ -1016,17 +1040,17 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H12" s="8" t="b">
         <v>1</v>
@@ -1055,16 +1079,16 @@
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="b">
@@ -1094,17 +1118,17 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H14" s="8" t="b">
         <v>1</v>
@@ -1133,16 +1157,16 @@
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="b">
@@ -1172,17 +1196,17 @@
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H16" s="8" t="b">
         <v>1</v>
@@ -1209,7 +1233,7 @@
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1224,7 +1248,7 @@
     </row>
     <row r="21" spans="2:10" ht="163.5" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>2</v>
@@ -1233,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>3</v>
@@ -1245,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1253,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D22" s="7" t="b">
         <v>1</v>
@@ -1277,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D23" s="7" t="b">
         <v>1</v>
@@ -1286,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="8">
@@ -1301,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D24" s="7" t="b">
         <v>1</v>
@@ -1325,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D25" s="7" t="b">
         <v>1</v>
@@ -1334,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="8">
@@ -1349,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D26" s="7" t="b">
         <v>1</v>
@@ -1361,7 +1385,7 @@
         <v>8</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H26" s="8">
         <v>1</v>
@@ -1375,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D27" s="7" t="b">
         <v>1</v>
@@ -1384,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="8">
@@ -1399,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D28" s="7" t="b">
         <v>1</v>
@@ -1411,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H28" s="8">
         <v>1</v>
@@ -1423,7 +1447,7 @@
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1436,12 +1460,12 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J34" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="118.5" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>2</v>
@@ -1453,7 +1477,7 @@
         <v>3</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>1</v>
@@ -1462,46 +1486,44 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K35" s="17"/>
     </row>
-    <row r="36" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="D36" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F36" s="12"/>
       <c r="G36" s="8" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="H36" s="8">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I36" s="8">
-        <v>1</v>
+        <v>10080</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1514,22 +1536,22 @@
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F40" s="14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G40" s="14"/>
       <c r="H40" s="14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="2:11" ht="155.25" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>3</v>
@@ -1541,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1549,10 +1571,10 @@
         <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>5</v>
@@ -1562,7 +1584,7 @@
         <v>25000</v>
       </c>
       <c r="H42" s="12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I42" s="2"/>
     </row>
@@ -1571,22 +1593,22 @@
         <v>0</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G43" s="12">
         <v>1</v>
       </c>
       <c r="H43" s="12">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1594,10 +1616,10 @@
         <v>0</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>7</v>
@@ -1607,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="H44" s="12">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1615,22 +1637,22 @@
         <v>0</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G45" s="12">
         <v>1</v>
       </c>
       <c r="H45" s="12">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1661,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5 D22:D28 D42:D45 D36 D11:D16"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5 D22:D28 D11:D16 D36"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
enable Welcome back feature to FALSE to ensure nobody can see it until we activate it in CRM
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
+++ b/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
@@ -821,7 +821,7 @@
   <dimension ref="B1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8">
         <v>4</v>

</xml_diff>

<commit_message>
Welcome Back - Refactor: rename parameter "duration"
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
+++ b/Docs/Content/HungryDragonContent_WelcomeBack.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdiez\Documents\client_lfs\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/clientlfs/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F86E79-917F-4948-9821-6F31B87EF467}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="18360" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25400" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -101,9 +102,6 @@
     <t>[target]</t>
   </si>
   <si>
-    <t>[duration]</t>
-  </si>
-  <si>
     <t>[description]</t>
   </si>
   <si>
@@ -276,12 +274,15 @@
   </si>
   <si>
     <t>CLUSTER_GENERIC</t>
+  </si>
+  <si>
+    <t>[durationMinutes]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,34 +818,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -854,9 +855,9 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="4" spans="2:15" ht="170.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="167" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -865,13 +866,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>12</v>
@@ -898,7 +899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -918,13 +919,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="8">
         <v>7</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K5" s="8">
         <v>10080</v>
@@ -942,10 +943,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:15" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -955,9 +956,9 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="10" spans="2:15" s="17" customFormat="1" ht="152.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" s="17" customFormat="1" ht="148" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>2</v>
@@ -966,51 +967,51 @@
         <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="b">
@@ -1035,22 +1036,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="8" t="b">
         <v>1</v>
@@ -1074,21 +1075,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="b">
@@ -1113,22 +1114,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="8" t="b">
         <v>1</v>
@@ -1152,21 +1153,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="b">
@@ -1191,22 +1192,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="8" t="b">
         <v>1</v>
@@ -1230,10 +1231,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:10" ht="24" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1243,12 +1244,12 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="2:10" ht="163.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="161" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>2</v>
@@ -1257,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>3</v>
@@ -1269,15 +1270,15 @@
         <v>4</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="7" t="b">
         <v>1</v>
@@ -1296,12 +1297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="7" t="b">
         <v>1</v>
@@ -1310,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="8">
@@ -1320,12 +1321,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="7" t="b">
         <v>1</v>
@@ -1344,12 +1345,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="7" t="b">
         <v>1</v>
@@ -1358,7 +1359,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="8">
@@ -1368,12 +1369,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="7" t="b">
         <v>1</v>
@@ -1385,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H26" s="8">
         <v>1</v>
@@ -1394,12 +1395,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="7" t="b">
         <v>1</v>
@@ -1408,7 +1409,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="8">
@@ -1418,12 +1419,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" s="7" t="b">
         <v>1</v>
@@ -1435,7 +1436,7 @@
         <v>8</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H28" s="8">
         <v>1</v>
@@ -1444,8 +1445,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1458,14 +1459,14 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J34" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="118.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="116" x14ac:dyDescent="0.2">
       <c r="B35" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>2</v>
@@ -1486,29 +1487,29 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="K35" s="17"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="D36" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H36" s="8">
         <v>32</v>
@@ -1517,13 +1518,13 @@
         <v>10080</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:11" ht="24" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1534,24 +1535,24 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F40" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" s="14"/>
       <c r="H40" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="155.25" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="152" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>3</v>
@@ -1566,15 +1567,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>5</v>
@@ -1588,21 +1589,21 @@
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G43" s="12">
         <v>1</v>
@@ -1611,15 +1612,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>7</v>
@@ -1632,21 +1633,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B45" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G45" s="12">
         <v>1</v>
@@ -1656,12 +1657,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B10:N10"/>
+  <autoFilter ref="B10:N10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="G26 G28">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5 D22:D28 D11:D16 D36"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5 D22:D28 D11:D16 D36" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>